<commit_message>
small change is implemented.
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/design.xlsx
+++ b/libalconcurrent/doc/design.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work_space\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C696C2-D7D8-48A4-9D0C-5DF82EC4CD1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51D4E3E-6A51-46B9-841E-9A406BEB8208}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Inside structure" sheetId="1" r:id="rId1"/>
+    <sheet name="Layering of software module" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -162,7 +163,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>Semi-lock free data structure</a:t>
+            <a:t>Semi lock-free data structure</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
@@ -626,8 +627,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4111335" y="6070889"/>
-          <a:ext cx="3044538" cy="4421331"/>
+          <a:off x="4076699" y="5962650"/>
+          <a:ext cx="3009901" cy="4343400"/>
           <a:chOff x="2181224" y="1485900"/>
           <a:chExt cx="3009901" cy="4343400"/>
         </a:xfrm>
@@ -1736,8 +1737,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3237633" y="3432463"/>
-          <a:ext cx="2532785" cy="1659082"/>
+          <a:off x="3209924" y="3371849"/>
+          <a:ext cx="2505076" cy="1628776"/>
           <a:chOff x="2362199" y="2257424"/>
           <a:chExt cx="2505076" cy="1628776"/>
         </a:xfrm>
@@ -2589,8 +2590,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11188410" y="1364672"/>
-          <a:ext cx="12456765" cy="12888192"/>
+          <a:off x="11077574" y="1343024"/>
+          <a:ext cx="12332074" cy="12658726"/>
           <a:chOff x="8534399" y="1343024"/>
           <a:chExt cx="12417799" cy="12658726"/>
         </a:xfrm>
@@ -8149,6 +8150,1224 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAFC22E6-6FAE-42C8-A9AA-EBE770D8C165}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3276601" y="3962400"/>
+          <a:ext cx="3429000" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>Lock-free FIFO queue</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B64C21F4-8DD8-4AC3-8E53-BE881BA625B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7010401" y="3971925"/>
+          <a:ext cx="3429000" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>Lock-free Stack</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>504826</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>504826</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AE36994-21C2-4797-AE08-03E96BF63BC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10791826" y="3971925"/>
+          <a:ext cx="3429000" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>Lock-free List</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51C1508D-167F-4867-9C28-C85952DDAE67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5153026" y="1352550"/>
+          <a:ext cx="3429000" cy="819150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>One</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
+            <a:t> side deque</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直線矢印コネクタ 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAF90EE7-9242-47F9-BC38-7018AA0B4E96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="2" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4991101" y="2247900"/>
+          <a:ext cx="1171574" cy="1714500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495301</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直線矢印コネクタ 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5330FA23-062E-4ADB-9AFB-C0819C3AACF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="3" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7391400" y="2247900"/>
+          <a:ext cx="1333501" cy="1724025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>109969</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="正方形/長方形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CD44041-9941-4265-890A-18DC095CA93C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7032049" y="11020424"/>
+          <a:ext cx="3463636" cy="836469"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>Dynamic</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
+            <a:t> local strage</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>108239</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>86591</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>223405</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="正方形/長方形 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9476B1B-3CC7-4BF9-8D1A-BD544F3189E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4957330" y="9085118"/>
+          <a:ext cx="7598352" cy="836469"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>Hazard</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
+            <a:t> Pointer</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>468457</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>128155</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>468457</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>237260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="正方形/長方形 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EF51237-7753-4266-86A5-01FDBFCC2582}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8088457" y="7401791"/>
+          <a:ext cx="3463636" cy="836469"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>base</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
+            <a:t> lock-free node for list structure</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>516947</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>159326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>516946</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>25977</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="正方形/長方形 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{307E24EC-96D5-41B4-9B79-EA077E8B41F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3980583" y="5735781"/>
+          <a:ext cx="3463636" cy="836469"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>Free</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
+            <a:t> node strage</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>170583</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>25977</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>443779</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="直線矢印コネクタ 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{725675D8-1030-4EAA-A85A-B510A2B68C11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="15" idx="2"/>
+          <a:endCxn id="13" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5712401" y="6572250"/>
+          <a:ext cx="3044105" cy="2512868"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>443779</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>237260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>122093</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="直線矢印コネクタ 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8F60E35-7EAF-4C47-B244-E85F5FB2CFA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="2"/>
+          <a:endCxn id="13" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8756506" y="8238260"/>
+          <a:ext cx="1063769" cy="846858"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>467591</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>122093</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>128155</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="直線矢印コネクタ 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{171E5C0A-0B16-43CE-B193-76C9BFA5EEC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="14" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6702136" y="6650182"/>
+          <a:ext cx="3118139" cy="751609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>443779</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>223405</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>451140</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>109969</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="直線矢印コネクタ 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62832691-528B-4D44-A95D-80A2CB1AE03E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="13" idx="2"/>
+          <a:endCxn id="12" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8756506" y="9921587"/>
+          <a:ext cx="7361" cy="1098837"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>122093</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>158462</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>128155</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="直線矢印コネクタ 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC1D47AD-71B3-4271-847B-AC52A4AC262A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="14" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9820275" y="4877666"/>
+          <a:ext cx="2807278" cy="2524125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>498765</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>122093</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>128155</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="直線矢印コネクタ 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C643C78E-C438-4F7B-A7F4-A5EBEF9A83A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="14" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8811492" y="4877666"/>
+          <a:ext cx="1008783" cy="2524125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>187037</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>122093</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>128155</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="直線矢印コネクタ 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE742BF1-B20F-4294-ADC8-98CF29C1D632}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="14" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5036128" y="4868141"/>
+          <a:ext cx="4784147" cy="2533650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>187037</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>170583</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>159326</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="直線矢印コネクタ 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{939BE6E8-E827-4486-B198-1818F6F7BD53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="15" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5036128" y="4868141"/>
+          <a:ext cx="676273" cy="867640"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>170583</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>498765</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>159326</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="直線矢印コネクタ 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE7A4FE6-B7BA-4CE1-ABAC-09C057179B36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="15" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5712401" y="4877666"/>
+          <a:ext cx="3099091" cy="858115"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>170583</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>158462</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>159326</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="直線矢印コネクタ 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D447743-3D60-440E-8A62-31B0088F941A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="15" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5712401" y="4877666"/>
+          <a:ext cx="6915152" cy="858115"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8414,8 +9633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -8451,4 +9670,21 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D562D89-000B-4917-9793-91D28449AAD1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test: update test case
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/design.xlsx
+++ b/libalconcurrent/doc/design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0257F2FD-E702-4AB4-AE2B-A5FF5C14E4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FFA5FF-052F-4BCF-8862-2B7D8086666E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9791,13 +9791,13 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>667718</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>19918</xdr:rowOff>
+      <xdr:rowOff>71872</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>667718</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>129023</xdr:rowOff>
+      <xdr:rowOff>180977</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9812,7 +9812,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11058627" y="15537009"/>
+          <a:off x="11058627" y="15588963"/>
           <a:ext cx="3463636" cy="836469"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9861,7 +9861,7 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>321354</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>19918</xdr:rowOff>
+      <xdr:rowOff>71872</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9880,7 +9880,121 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8751720" y="14316078"/>
-          <a:ext cx="4038725" cy="1220931"/>
+          <a:ext cx="4038725" cy="1272885"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>2038</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>139874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>321354</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>71872</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直線矢印コネクタ 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A901EBE-CA54-4C0C-AA99-6A265424B6BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="13" idx="2"/>
+          <a:endCxn id="8" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9700220" y="12262601"/>
+          <a:ext cx="3090225" cy="3326362"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>321354</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>121890</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>511625</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>71872</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直線矢印コネクタ 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B5A15F7-CEAA-4AFD-9B7B-62EEDF5F8081}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="47" idx="2"/>
+          <a:endCxn id="8" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12790445" y="10547435"/>
+          <a:ext cx="1575725" cy="5041528"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10218,8 +10332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D562D89-000B-4917-9793-91D28449AAD1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Y65" sqref="Y65"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AC68" sqref="AC68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>

<commit_message>
doc: fix missing keyward
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/design.xlsx
+++ b/libalconcurrent/doc/design.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18FFA5FF-052F-4BCF-8862-2B7D8086666E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAD358B-3863-40AB-8649-FBA0BE2A22E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8584,7 +8584,7 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
-            <a:t> local strage</a:t>
+            <a:t> thread local strage</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
         </a:p>
@@ -10332,8 +10332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D562D89-000B-4917-9793-91D28449AAD1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AC68" sqref="AC68"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AC57" sqref="AC57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>

<commit_message>
refactor: make node class that is usable generally with hazard pointer handler
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/design.xlsx
+++ b/libalconcurrent/doc/design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAD358B-3863-40AB-8649-FBA0BE2A22E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5F24CA-425F-4A1D-8661-C53FD13A45A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8528,13 +8528,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>250454</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>144609</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>627530</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>11260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8594,16 +8594,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>211894</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>37899</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>471666</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>176445</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>484909</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>139874</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>51954</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>35965</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8618,7 +8618,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8524621" y="11433263"/>
+          <a:off x="15711666" y="19815263"/>
           <a:ext cx="2351197" cy="829338"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8662,16 +8662,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>468457</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>128155</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>174048</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>110837</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>468457</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>237260</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>174047</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>219942</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8686,8 +8686,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8088457" y="7401791"/>
-          <a:ext cx="3463636" cy="836469"/>
+          <a:off x="6408593" y="14658110"/>
+          <a:ext cx="3463636" cy="836468"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8715,12 +8715,8 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
-            <a:t>base</a:t>
-          </a:r>
-          <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
-            <a:t> lock-free node for list structure</a:t>
+            <a:t>node of one direction list structure</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
         </a:p>
@@ -8730,16 +8726,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>516947</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>159326</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>482311</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>72736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>516946</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>25977</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>482310</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>181842</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8754,7 +8750,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3980583" y="5735781"/>
+          <a:off x="14336856" y="8801100"/>
           <a:ext cx="3463636" cy="836469"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8798,16 +8794,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>170583</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>25977</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>135947</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>181842</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>2038</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>37899</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>261810</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>176445</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8825,8 +8821,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5712401" y="6572250"/>
-          <a:ext cx="3987819" cy="4861013"/>
+          <a:off x="16068674" y="9637569"/>
+          <a:ext cx="818591" cy="10177694"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8855,16 +8851,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>2038</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>237260</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>158462</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>122093</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>37899</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>336967</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>242452</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8876,14 +8872,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="14" idx="2"/>
-          <a:endCxn id="13" idx="0"/>
+          <a:cxnSpLocks/>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="11" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="9700220" y="8238260"/>
-          <a:ext cx="120055" cy="3195003"/>
+        <a:xfrm>
+          <a:off x="12627553" y="4877666"/>
+          <a:ext cx="871232" cy="7729968"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8912,16 +8909,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>467591</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>103909</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520411</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>181842</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>122093</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>128155</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>135947</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>110837</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8933,13 +8930,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:stCxn id="15" idx="2"/>
           <a:endCxn id="14" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6702136" y="6650182"/>
-          <a:ext cx="3118139" cy="751609"/>
+        <a:xfrm flipH="1">
+          <a:off x="8140411" y="9637569"/>
+          <a:ext cx="7928263" cy="5020541"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8968,73 +8966,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>438993</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>139874</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>2038</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>144609</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="直線矢印コネクタ 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62832691-528B-4D44-A95D-80A2CB1AE03E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="13" idx="2"/>
-          <a:endCxn id="12" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="8751720" y="12262601"/>
-          <a:ext cx="948500" cy="1217008"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="diamond" w="lg" len="lg"/>
-          <a:tailEnd type="none"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>122093</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520411</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>158462</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>128155</xdr:rowOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>110837</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9052,8 +8993,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9820275" y="4877666"/>
-          <a:ext cx="2807278" cy="2524125"/>
+          <a:off x="8140411" y="4877666"/>
+          <a:ext cx="4487142" cy="9780444"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9082,16 +9023,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>498765</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520411</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>122093</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>128155</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>498765</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>110837</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9108,9 +9049,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8811492" y="4877666"/>
-          <a:ext cx="1008783" cy="2524125"/>
+        <a:xfrm flipH="1">
+          <a:off x="8140411" y="4877666"/>
+          <a:ext cx="671081" cy="9780444"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9145,10 +9086,10 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>122093</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>128155</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520411</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>110837</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9167,7 +9108,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5036128" y="4868141"/>
-          <a:ext cx="4784147" cy="2533650"/>
+          <a:ext cx="3104283" cy="9789969"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9202,10 +9143,10 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>170583</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>159326</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>135947</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>72736</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9224,7 +9165,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5036128" y="4868141"/>
-          <a:ext cx="676273" cy="867640"/>
+          <a:ext cx="11032546" cy="3932959"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9253,16 +9194,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>170583</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>498765</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>498765</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>159326</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>135947</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>72736</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9279,9 +9220,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5712401" y="4877666"/>
-          <a:ext cx="3099091" cy="858115"/>
+        <a:xfrm>
+          <a:off x="8811492" y="4877666"/>
+          <a:ext cx="7257182" cy="3923434"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9310,16 +9251,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>170583</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>158462</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>158462</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>159326</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>135947</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>72736</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9336,9 +9277,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5712401" y="4877666"/>
-          <a:ext cx="6915152" cy="858115"/>
+        <a:xfrm>
+          <a:off x="12627553" y="4877666"/>
+          <a:ext cx="3441121" cy="3923434"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9369,14 +9310,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>96218</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>54554</xdr:rowOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>106508</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>96218</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>163659</xdr:rowOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>215614</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9391,7 +9332,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7023491" y="15571645"/>
+          <a:off x="7023491" y="24351963"/>
           <a:ext cx="3463636" cy="836469"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9437,14 +9378,14 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>438993</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>11260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>442582</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>54554</xdr:rowOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>106508</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9462,8 +9403,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8751720" y="14316078"/>
-          <a:ext cx="3589" cy="1255567"/>
+          <a:off x="8751720" y="20619896"/>
+          <a:ext cx="3589" cy="3732067"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9492,73 +9433,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>170583</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>25977</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>438993</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>144609</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="44" name="直線矢印コネクタ 43">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF613727-3177-44A1-84DB-ADDC709B6C67}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="15" idx="2"/>
-          <a:endCxn id="12" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5712401" y="6572250"/>
-          <a:ext cx="3039319" cy="6907359"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:headEnd type="diamond" w="lg" len="lg"/>
-          <a:tailEnd type="none"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>122705</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>659569</xdr:colOff>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>19915</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>207816</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>121890</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>51953</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>121891</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9573,8 +9457,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12591796" y="9718097"/>
-          <a:ext cx="3548747" cy="829338"/>
+          <a:off x="7586842" y="17719097"/>
+          <a:ext cx="3548747" cy="829339"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9619,13 +9503,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>438993</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>121890</xdr:rowOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>121891</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>511625</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>355761</xdr:colOff>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>144609</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9644,8 +9528,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8751720" y="10547435"/>
-          <a:ext cx="5614450" cy="2932174"/>
+          <a:off x="8751720" y="18548436"/>
+          <a:ext cx="609496" cy="1234991"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9674,16 +9558,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>2038</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>121890</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>355761</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>121891</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>511625</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>37899</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>261810</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>176445</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9700,9 +9584,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="9700220" y="10547435"/>
-          <a:ext cx="4665950" cy="885828"/>
+        <a:xfrm>
+          <a:off x="9361216" y="18548436"/>
+          <a:ext cx="7526049" cy="1266827"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9731,15 +9615,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>122093</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>237260</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520411</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>219942</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>511625</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>355761</xdr:colOff>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>19915</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9758,8 +9642,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9820275" y="8238260"/>
-          <a:ext cx="4545895" cy="1479837"/>
+          <a:off x="8140411" y="15494578"/>
+          <a:ext cx="1220805" cy="2224519"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9790,13 +9674,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>667718</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>71872</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>667718</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>180977</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9842,7 +9726,15 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
-            <a:t>allocate_only_mem</a:t>
+            <a:t>allocate_only_mem(semi</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
+            <a:t> lock-free</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
         </a:p>
@@ -9854,13 +9746,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>438993</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>11260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>321354</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>71872</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9909,15 +9801,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>2038</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>139874</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>321354</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>35965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>321354</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>261810</xdr:colOff>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>71872</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9935,9 +9827,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9700220" y="12262601"/>
-          <a:ext cx="3090225" cy="3326362"/>
+        <a:xfrm flipH="1">
+          <a:off x="12790445" y="20644601"/>
+          <a:ext cx="4096820" cy="1248180"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9966,15 +9858,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>355761</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>121891</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>321354</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>121890</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>511625</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>71872</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9992,9 +9884,606 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9361216" y="18548436"/>
+          <a:ext cx="3429229" cy="3344345"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>640775</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>242452</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>33158</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>101972</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="正方形/長方形 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7A1985B-55A7-48D3-80FD-743571C94C2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11724411" y="12607634"/>
+          <a:ext cx="3548747" cy="829338"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>retire</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
+            <a:t> manager module</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>336967</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>101972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>261810</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>176445</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="直線矢印コネクタ 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BF45EEF-2BB1-4841-B429-B9C0C1D33BB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="2"/>
+          <a:endCxn id="13" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13498785" y="13436972"/>
+          <a:ext cx="3388480" cy="6378291"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520411</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>101972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>336967</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>110837</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="直線矢印コネクタ 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA1DBFF5-BB13-4D4C-9230-69BAD4954836}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="11" idx="2"/>
+          <a:endCxn id="14" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="12790445" y="10547435"/>
-          <a:ext cx="1575725" cy="5041528"/>
+          <a:off x="8140411" y="13436972"/>
+          <a:ext cx="5358374" cy="1221138"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>144709</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>103044</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>144709</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>212150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="正方形/長方形 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{071B79CF-71EA-43C3-8418-B69AC843B376}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15384709" y="24348499"/>
+          <a:ext cx="3463636" cy="836469"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000" baseline="0"/>
+            <a:t>thread local memory</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>261810</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>35965</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>491072</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>103044</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="直線矢印コネクタ 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FEAC810-901D-4171-BB31-03C1A57A24D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="13" idx="2"/>
+          <a:endCxn id="59" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16887265" y="20644601"/>
+          <a:ext cx="229262" cy="3703898"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>26946</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>26945</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>232932</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="正方形/長方形 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{162AF38A-E922-4654-B326-EE07686F3863}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11110582" y="24369281"/>
+          <a:ext cx="3463636" cy="836469"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>mmap</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>321354</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>180977</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>373309</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="直線矢印コネクタ 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACA13337-C964-47A0-9824-2CFF661EC87F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="2"/>
+          <a:endCxn id="65" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12790445" y="22729250"/>
+          <a:ext cx="51955" cy="1640031"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>498765</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>336967</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>242452</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="96" name="直線矢印コネクタ 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4381AAE6-BCE7-4403-8960-7435A1A2EF0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="11" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8811492" y="4877666"/>
+          <a:ext cx="4687293" cy="7729968"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>187037</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>336967</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>242452</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="100" name="直線矢印コネクタ 99">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A8CB120-CD5D-4059-AF98-A2D294C4CF79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="2" idx="2"/>
+          <a:endCxn id="11" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5036128" y="4868141"/>
+          <a:ext cx="8462657" cy="7739493"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="diamond" w="lg" len="lg"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520411</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>219942</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>261810</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>176445</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="124" name="直線矢印コネクタ 123">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F43F36BA-57CD-4E1C-9FE6-DAD8439633AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="2"/>
+          <a:endCxn id="13" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8140411" y="15494578"/>
+          <a:ext cx="8746854" cy="4320685"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10332,8 +10821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D562D89-000B-4917-9793-91D28449AAD1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AC57" sqref="AC57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AD61" sqref="AD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>